<commit_message>
Figures updated using moderated ANCOM-BC.
</commit_message>
<xml_diff>
--- a/tables/Supplementary Table 1.xlsx
+++ b/tables/Supplementary Table 1.xlsx
@@ -76,9 +76,6 @@
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">p__Firmicutes</t>
-  </si>
-  <si>
     <t xml:space="preserve">p__Actinobacteria</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">p__Euryarchaeota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p__Firmicutes</t>
   </si>
   <si>
     <t xml:space="preserve">p__Proteobacteria</t>
@@ -536,19 +536,19 @@
         <v>2.60071295144874</v>
       </c>
       <c r="C4" t="n">
-        <v>0.243252630064134</v>
+        <v>0.317869614947217</v>
       </c>
       <c r="D4" t="n">
-        <v>1.89758841207969</v>
+        <v>1.68190715465118</v>
       </c>
       <c r="E4" t="n">
-        <v>3.30383749081779</v>
+        <v>3.5195187482463</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.000000000000000000000000122829949292203</v>
+        <v>0.00000000000000307860874311449</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
@@ -565,19 +565,19 @@
         <v>-4.03494743799976</v>
       </c>
       <c r="C5" t="n">
-        <v>0.519849098810269</v>
+        <v>0.594466083693352</v>
       </c>
       <c r="D5" t="n">
-        <v>-5.53757726792603</v>
+        <v>-5.75325852535454</v>
       </c>
       <c r="E5" t="n">
-        <v>-2.53231760807349</v>
+        <v>-2.31663635064498</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0000000000000921297884289652</v>
+        <v>0.00000000012548957399238</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -594,19 +594,19 @@
         <v>2.9496919912475</v>
       </c>
       <c r="C6" t="n">
-        <v>0.40001768929904</v>
+        <v>0.474634674182123</v>
       </c>
       <c r="D6" t="n">
-        <v>1.79343623584742</v>
+        <v>1.57775497841891</v>
       </c>
       <c r="E6" t="n">
-        <v>4.10594774664757</v>
+        <v>4.32162900407608</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.00000000000182272946987786</v>
+        <v>0.00000000565803499410997</v>
       </c>
       <c r="H6" t="s">
         <v>10</v>
@@ -623,19 +623,19 @@
         <v>-2.74817450638746</v>
       </c>
       <c r="C7" t="n">
-        <v>0.449225148399104</v>
+        <v>0.523842133282187</v>
       </c>
       <c r="D7" t="n">
-        <v>-4.04666499118853</v>
+        <v>-4.26234624861704</v>
       </c>
       <c r="E7" t="n">
-        <v>-1.44968402158639</v>
+        <v>-1.23400276415788</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0000000104502342082608</v>
+        <v>0.00000170805960394475</v>
       </c>
       <c r="H7" t="s">
         <v>10</v>
@@ -652,19 +652,19 @@
         <v>0.513945333391076</v>
       </c>
       <c r="C8" t="n">
-        <v>0.212507013930058</v>
+        <v>0.287123998813141</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.100308647101836</v>
+        <v>-0.315989904530348</v>
       </c>
       <c r="E8" t="n">
-        <v>1.12819931388399</v>
+        <v>1.3438805713125</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.17143748681751</v>
+        <v>0.808033825622582</v>
       </c>
       <c r="H8" t="s">
         <v>10</v>
@@ -678,22 +678,22 @@
         <v>19</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.32146839584504</v>
+        <v>0.646306806016922</v>
       </c>
       <c r="C9" t="n">
-        <v>0.156114483841846</v>
+        <v>0.451839817125758</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.772719116181318</v>
+        <v>-0.659741408965922</v>
       </c>
       <c r="E9" t="n">
-        <v>0.129782324491239</v>
+        <v>1.95235502099977</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.434243115651438</v>
+        <v>1</v>
       </c>
       <c r="H9" t="s">
         <v>10</v>
@@ -707,22 +707,22 @@
         <v>20</v>
       </c>
       <c r="B10" t="n">
-        <v>0.646306806016922</v>
+        <v>0.846152719012753</v>
       </c>
       <c r="C10" t="n">
-        <v>0.377222832242675</v>
+        <v>0.582853971281676</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.444060151537411</v>
+        <v>-0.838593423172023</v>
       </c>
       <c r="E10" t="n">
-        <v>1.73667376357125</v>
+        <v>2.53089886119753</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.953172395146093</v>
+        <v>1</v>
       </c>
       <c r="H10" t="s">
         <v>10</v>
@@ -736,16 +736,16 @@
         <v>21</v>
       </c>
       <c r="B11" t="n">
-        <v>0.846152719012753</v>
+        <v>-0.117255159131472</v>
       </c>
       <c r="C11" t="n">
-        <v>0.508236986398594</v>
+        <v>0.235242787862366</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.622912165743511</v>
+        <v>-0.797227157016996</v>
       </c>
       <c r="E11" t="n">
-        <v>2.31521760376902</v>
+        <v>0.562716838754051</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -765,16 +765,16 @@
         <v>22</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.117255159131472</v>
+        <v>-0.32146839584504</v>
       </c>
       <c r="C12" t="n">
-        <v>0.160625802979283</v>
+        <v>0.230731468724928</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.581545899588485</v>
+        <v>-0.988400373609829</v>
       </c>
       <c r="E12" t="n">
-        <v>0.34703558132554</v>
+        <v>0.34546358191975</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -797,13 +797,13 @@
         <v>-0.363821014724214</v>
       </c>
       <c r="C13" t="n">
-        <v>0.36095905980986</v>
+        <v>0.435576044692943</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.40717735004104</v>
+        <v>-1.62285860746955</v>
       </c>
       <c r="E13" t="n">
-        <v>0.679535320592608</v>
+        <v>0.895216578021119</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -826,13 +826,13 @@
         <v>0.0429564155560438</v>
       </c>
       <c r="C14" t="n">
-        <v>0.17945714971842</v>
+        <v>0.254074134601503</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.475766550353838</v>
+        <v>-0.69144780778235</v>
       </c>
       <c r="E14" t="n">
-        <v>0.561679381465926</v>
+        <v>0.777360638894437</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -1014,19 +1014,19 @@
         <v>6.25623454531064</v>
       </c>
       <c r="C5" t="n">
-        <v>0.523087230142417</v>
+        <v>0.957108005020814</v>
       </c>
       <c r="D5" t="n">
-        <v>4.73210151606007</v>
+        <v>3.46748376159302</v>
       </c>
       <c r="E5" t="n">
-        <v>7.78036757456121</v>
+        <v>9.04498532902826</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0000000000000000000000000000000631561162884799</v>
+        <v>0.000000000692252311891259</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
@@ -1043,193 +1043,193 @@
         <v>-4.26076892184244</v>
       </c>
       <c r="C6" t="n">
-        <v>0.657080568416928</v>
+        <v>1.09110134329533</v>
       </c>
       <c r="D6" t="n">
-        <v>-6.17532186730493</v>
+        <v>-7.43993962177198</v>
       </c>
       <c r="E6" t="n">
-        <v>-2.34621597637995</v>
+        <v>-1.0815982219129</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.000000000979984149253423</v>
+        <v>0.00103640783997099</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.90948397329009</v>
+        <v>3.55358160279929</v>
       </c>
       <c r="C7" t="n">
-        <v>0.327947613564495</v>
+        <v>1.08596539359687</v>
       </c>
       <c r="D7" t="n">
-        <v>-2.8650335659679</v>
+        <v>0.389375654675779</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.953934380612283</v>
+        <v>6.7177875509228</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0000000637607134769436</v>
+        <v>0.0117352722684026</v>
       </c>
       <c r="H7" t="s">
         <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B8" t="n">
-        <v>3.55358160279929</v>
+        <v>3.06690070843383</v>
       </c>
       <c r="C8" t="n">
-        <v>0.651944618718474</v>
+        <v>1.05340860543981</v>
       </c>
       <c r="D8" t="n">
-        <v>1.65399340914283</v>
+        <v>-0.00244366919600925</v>
       </c>
       <c r="E8" t="n">
-        <v>5.45316979645576</v>
+        <v>6.13624508606367</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.00000055176253185185</v>
+        <v>0.0395786076941127</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" t="n">
-        <v>3.06690070843383</v>
+        <v>-1.90948397329009</v>
       </c>
       <c r="C9" t="n">
-        <v>0.61938783056141</v>
+        <v>0.761968388442892</v>
       </c>
       <c r="D9" t="n">
-        <v>1.26217408527104</v>
+        <v>-4.12965132043495</v>
       </c>
       <c r="E9" t="n">
-        <v>4.87162733159662</v>
+        <v>0.310683373854766</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.00000810067278349778</v>
+        <v>0.134320573116715</v>
       </c>
       <c r="H9" t="s">
         <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" t="n">
-        <v>1.17466221039992</v>
+        <v>0.10610149948576</v>
       </c>
       <c r="C10" t="n">
-        <v>0.279612295989963</v>
+        <v>0.703997381356196</v>
       </c>
       <c r="D10" t="n">
-        <v>0.359948504644077</v>
+        <v>-1.94515419861024</v>
       </c>
       <c r="E10" t="n">
-        <v>1.98937591615577</v>
+        <v>2.15735719758176</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.000292261862215732</v>
+        <v>1</v>
       </c>
       <c r="H10" t="s">
         <v>26</v>
       </c>
       <c r="I10" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.747832996345051</v>
+        <v>-0.62157578854071</v>
       </c>
       <c r="C11" t="n">
-        <v>0.222236147680543</v>
+        <v>0.653567945591162</v>
       </c>
       <c r="D11" t="n">
-        <v>-1.39536830872709</v>
+        <v>-2.52589391242938</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.100297683963016</v>
+        <v>1.28274233534796</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00841865471512599</v>
+        <v>1</v>
       </c>
       <c r="H11" t="s">
         <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.62157578854071</v>
+        <v>0.870330512046186</v>
       </c>
       <c r="C12" t="n">
-        <v>0.219547170712765</v>
+        <v>0.916654644119761</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.26127615796233</v>
+        <v>-1.80055024934896</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0181245808809136</v>
+        <v>3.54121127344133</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0510155612256206</v>
+        <v>1</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
@@ -1240,25 +1240,25 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B13" t="n">
-        <v>0.870330512046186</v>
+        <v>1.17466221039992</v>
       </c>
       <c r="C13" t="n">
-        <v>0.482633869241364</v>
+        <v>0.71363307086836</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.535932494881909</v>
+        <v>-0.904669249822971</v>
       </c>
       <c r="E13" t="n">
-        <v>2.27659351897428</v>
+        <v>3.25399367062282</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0.784763487986671</v>
+        <v>1</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
@@ -1269,19 +1269,19 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>0.10610149948576</v>
+        <v>-0.0842444756762468</v>
       </c>
       <c r="C14" t="n">
-        <v>0.269976606477799</v>
+        <v>0.669521340289233</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.680536444143195</v>
+        <v>-2.03504642556346</v>
       </c>
       <c r="E14" t="n">
-        <v>0.892739443114715</v>
+        <v>1.86655747421097</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -1298,19 +1298,19 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.0842444756762468</v>
+        <v>-0.747832996345051</v>
       </c>
       <c r="C15" t="n">
-        <v>0.235500565410835</v>
+        <v>0.656256922558941</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.770428671096416</v>
+        <v>-2.65998606319414</v>
       </c>
       <c r="E15" t="n">
-        <v>0.601939719743922</v>
+        <v>1.16432007050403</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -1434,19 +1434,19 @@
         <v>4.1685101478655</v>
       </c>
       <c r="C4" t="n">
-        <v>0.431670387459329</v>
+        <v>0.540782286471597</v>
       </c>
       <c r="D4" t="n">
-        <v>2.92076190250603</v>
+        <v>2.60537269700204</v>
       </c>
       <c r="E4" t="n">
-        <v>5.41625839322497</v>
+        <v>5.73164759872896</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00000000000000000000506518239572981</v>
+        <v>0.000000000000140259178742054</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
@@ -1463,19 +1463,19 @@
         <v>2.10996832913156</v>
       </c>
       <c r="C5" t="n">
-        <v>0.404272342113685</v>
+        <v>0.513384241125952</v>
       </c>
       <c r="D5" t="n">
-        <v>0.941414450584032</v>
+        <v>0.626025245080044</v>
       </c>
       <c r="E5" t="n">
-        <v>3.2785222076791</v>
+        <v>3.59391141318308</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00000197693474381255</v>
+        <v>0.0004353752159312</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -1492,71 +1492,71 @@
         <v>1.83129046738175</v>
       </c>
       <c r="C6" t="n">
-        <v>0.443364748797426</v>
+        <v>0.552476647809693</v>
       </c>
       <c r="D6" t="n">
-        <v>0.549739535379602</v>
+        <v>0.234350329875614</v>
       </c>
       <c r="E6" t="n">
-        <v>3.1128413993839</v>
+        <v>3.42823060488789</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.000398280552461057</v>
+        <v>0.0100918210950258</v>
       </c>
       <c r="H6" t="s">
         <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="n">
         <v>1.49086520407092</v>
       </c>
       <c r="C7" t="n">
-        <v>0.498442640433816</v>
+        <v>0.607554539446084</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0501109895552616</v>
+        <v>-0.265278215948726</v>
       </c>
       <c r="E7" t="n">
-        <v>2.93161941858658</v>
+        <v>3.24700862409057</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0305825290434145</v>
+        <v>0.155457065548552</v>
       </c>
       <c r="H7" t="s">
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="n">
         <v>-0.244262374583913</v>
       </c>
       <c r="C8" t="n">
-        <v>0.566988552502593</v>
+        <v>0.67610045151486</v>
       </c>
       <c r="D8" t="n">
-        <v>-1.88314934037253</v>
+        <v>-2.19853854587652</v>
       </c>
       <c r="E8" t="n">
-        <v>1.39462459120471</v>
+        <v>1.71001379670869</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -1573,19 +1573,19 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="n">
         <v>0.392631542156252</v>
       </c>
       <c r="C9" t="n">
-        <v>0.279094330758827</v>
+        <v>0.388206229771094</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.414093847425662</v>
+        <v>-0.729483052929649</v>
       </c>
       <c r="E9" t="n">
-        <v>1.19935693173817</v>
+        <v>1.51474613724215</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -1602,19 +1602,19 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B10" t="n">
         <v>-0.0916681019861905</v>
       </c>
       <c r="C10" t="n">
-        <v>0.17606360895703</v>
+        <v>0.285175507969297</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.600581999093594</v>
+        <v>-0.915971204597582</v>
       </c>
       <c r="E10" t="n">
-        <v>0.417245795121213</v>
+        <v>0.732635000625201</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -1637,13 +1637,13 @@
         <v>-0.0367122110826159</v>
       </c>
       <c r="C11" t="n">
-        <v>0.364633025126398</v>
+        <v>0.473744924138665</v>
       </c>
       <c r="D11" t="n">
-        <v>-1.09068818562047</v>
+        <v>-1.40607739112446</v>
       </c>
       <c r="E11" t="n">
-        <v>1.01726376345524</v>
+        <v>1.33265296895923</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -1666,13 +1666,13 @@
         <v>-0.130887533638454</v>
       </c>
       <c r="C12" t="n">
-        <v>0.489288542678894</v>
+        <v>0.598400441691161</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.54518172276581</v>
+        <v>-1.8605709282698</v>
       </c>
       <c r="E12" t="n">
-        <v>1.2834066554889</v>
+        <v>1.59879586099289</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -1695,13 +1695,13 @@
         <v>0.058655285470948</v>
       </c>
       <c r="C13" t="n">
-        <v>0.228306932831949</v>
+        <v>0.337418831844216</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.601268543265873</v>
+        <v>-0.916657748769861</v>
       </c>
       <c r="E13" t="n">
-        <v>0.718579114207769</v>
+        <v>1.03396831971176</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -1724,13 +1724,13 @@
         <v>-0.819900657033559</v>
       </c>
       <c r="C14" t="n">
-        <v>0.712541649012804</v>
+        <v>0.821653548025072</v>
       </c>
       <c r="D14" t="n">
-        <v>-2.87951053097943</v>
+        <v>-3.19489973648341</v>
       </c>
       <c r="E14" t="n">
-        <v>1.23970921691231</v>
+        <v>1.5550984224163</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -1877,25 +1877,25 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" t="n">
         <v>-2.28116311114461</v>
       </c>
       <c r="C4" t="n">
-        <v>0.168325499196663</v>
+        <v>0.351898043856357</v>
       </c>
       <c r="D4" t="n">
-        <v>-2.77161754820069</v>
+        <v>-3.30649770289925</v>
       </c>
       <c r="E4" t="n">
-        <v>-1.79070867408852</v>
+        <v>-1.25582851938997</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0000000000000000000000000000000000000000924011642295969</v>
+        <v>0.00000000108290656147483</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
@@ -1906,25 +1906,25 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-2.87261124480962</v>
+        <v>3.88050543051919</v>
       </c>
       <c r="C5" t="n">
-        <v>0.294669548585368</v>
+        <v>0.635089430400732</v>
       </c>
       <c r="D5" t="n">
-        <v>-3.7311976637345</v>
+        <v>2.03002864266461</v>
       </c>
       <c r="E5" t="n">
-        <v>-2.01402482588473</v>
+        <v>5.73098221837376</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00000000000000000000224467976400428</v>
+        <v>0.0000000119428849615354</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
@@ -1935,25 +1935,25 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B6" t="n">
-        <v>-2.02435170757185</v>
+        <v>-2.87261124480962</v>
       </c>
       <c r="C6" t="n">
-        <v>0.208273092526988</v>
+        <v>0.478242093245063</v>
       </c>
       <c r="D6" t="n">
-        <v>-2.63120249866862</v>
+        <v>-4.26607781843306</v>
       </c>
       <c r="E6" t="n">
-        <v>-1.41750091647508</v>
+        <v>-1.47914467118617</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0000000000000000000029821889743996</v>
+        <v>0.0000000227338268801947</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
@@ -1964,25 +1964,25 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="n">
-        <v>3.88050543051919</v>
+        <v>-4.27886174538928</v>
       </c>
       <c r="C7" t="n">
-        <v>0.451516885741037</v>
+        <v>0.775253628039198</v>
       </c>
       <c r="D7" t="n">
-        <v>2.56490879736317</v>
+        <v>-6.53773864479127</v>
       </c>
       <c r="E7" t="n">
-        <v>5.1961020636752</v>
+        <v>-2.01998484598729</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.000000000000000100463055691682</v>
+        <v>0.000000408410077974224</v>
       </c>
       <c r="H7" t="s">
         <v>26</v>
@@ -1993,25 +1993,25 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.7448313110769</v>
+        <v>-2.02435170757185</v>
       </c>
       <c r="C8" t="n">
-        <v>0.236341115848892</v>
+        <v>0.391845637186683</v>
       </c>
       <c r="D8" t="n">
-        <v>-2.43346464043032</v>
+        <v>-3.16608265336718</v>
       </c>
       <c r="E8" t="n">
-        <v>-1.05619798172348</v>
+        <v>-0.882620761776526</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.00000000000186158647494925</v>
+        <v>0.00000286686174126159</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
@@ -2022,25 +2022,25 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B9" t="n">
-        <v>-4.27886174538928</v>
+        <v>-1.7448313110769</v>
       </c>
       <c r="C9" t="n">
-        <v>0.591681083379503</v>
+        <v>0.419913660508586</v>
       </c>
       <c r="D9" t="n">
-        <v>-6.00285849009271</v>
+        <v>-2.96834479512888</v>
       </c>
       <c r="E9" t="n">
-        <v>-2.55486500068585</v>
+        <v>-0.521317827024919</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.00000000000572370181177212</v>
+        <v>0.000389979098703508</v>
       </c>
       <c r="H9" t="s">
         <v>26</v>
@@ -2057,25 +2057,25 @@
         <v>-2.10047574233186</v>
       </c>
       <c r="C10" t="n">
-        <v>0.351091370435364</v>
+        <v>0.534663915095059</v>
       </c>
       <c r="D10" t="n">
-        <v>-3.12345990850945</v>
+        <v>-3.65834006320801</v>
       </c>
       <c r="E10" t="n">
-        <v>-1.07749157615427</v>
+        <v>-0.542611421455714</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0000000263356074647622</v>
+        <v>0.00102534103083569</v>
       </c>
       <c r="H10" t="s">
         <v>26</v>
       </c>
       <c r="I10" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
@@ -2086,25 +2086,25 @@
         <v>2.68862406807983</v>
       </c>
       <c r="C11" t="n">
-        <v>0.510918804190958</v>
+        <v>0.694491348850653</v>
       </c>
       <c r="D11" t="n">
-        <v>1.19994650177673</v>
+        <v>0.66506634707817</v>
       </c>
       <c r="E11" t="n">
-        <v>4.17730163438293</v>
+        <v>4.71218178908149</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00000170688094053023</v>
+        <v>0.00129877278194209</v>
       </c>
       <c r="H11" t="s">
         <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12">
@@ -2115,42 +2115,42 @@
         <v>-1.1043314014521</v>
       </c>
       <c r="C12" t="n">
-        <v>0.233002997093271</v>
+        <v>0.416575541752966</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.78323836633354</v>
+        <v>-2.3181185210321</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.425424436570654</v>
+        <v>0.109455718127904</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.000025702091174214</v>
+        <v>0.0963117009539047</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
       </c>
       <c r="I12" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="n">
         <v>0.737240752555557</v>
       </c>
       <c r="C13" t="n">
-        <v>0.602000496717108</v>
+        <v>0.785573041376803</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.01682393837943</v>
+        <v>-1.55170409307798</v>
       </c>
       <c r="E13" t="n">
-        <v>2.49130544349054</v>
+        <v>3.0261855981891</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -2173,13 +2173,13 @@
         <v>0.186861675188612</v>
       </c>
       <c r="C14" t="n">
-        <v>0.549813383355224</v>
+        <v>0.733385928014918</v>
       </c>
       <c r="D14" t="n">
-        <v>-1.41514405006595</v>
+        <v>-1.95002420476451</v>
       </c>
       <c r="E14" t="n">
-        <v>1.78886740044317</v>
+        <v>2.32374755514173</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -2202,13 +2202,13 @@
         <v>-0.337196087243825</v>
       </c>
       <c r="C15" t="n">
-        <v>0.336327832241869</v>
+        <v>0.519900376901564</v>
       </c>
       <c r="D15" t="n">
-        <v>-1.3171633436353</v>
+        <v>-1.85204349833385</v>
       </c>
       <c r="E15" t="n">
-        <v>0.642771169147646</v>
+        <v>1.1776513238462</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -2332,19 +2332,19 @@
         <v>-2.97705281260192</v>
       </c>
       <c r="C4" t="n">
-        <v>0.563403817339593</v>
+        <v>0.645069794567981</v>
       </c>
       <c r="D4" t="n">
-        <v>-4.63075539801456</v>
+        <v>-4.8704613309998</v>
       </c>
       <c r="E4" t="n">
-        <v>-1.32335022718927</v>
+        <v>-1.08364429420403</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00000164268158201183</v>
+        <v>0.000051081145091242</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
@@ -2361,19 +2361,19 @@
         <v>-2.36911056677888</v>
       </c>
       <c r="C5" t="n">
-        <v>0.457727729913429</v>
+        <v>0.539393707141817</v>
       </c>
       <c r="D5" t="n">
-        <v>-3.71263275650634</v>
+        <v>-3.95233868949158</v>
       </c>
       <c r="E5" t="n">
-        <v>-1.02558837705142</v>
+        <v>-0.785882444066181</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00000295005716887245</v>
+        <v>0.00014589023435706</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -2390,25 +2390,25 @@
         <v>1.12619881795637</v>
       </c>
       <c r="C6" t="n">
-        <v>0.265837021367222</v>
+        <v>0.34750299859561</v>
       </c>
       <c r="D6" t="n">
-        <v>0.345914134034197</v>
+        <v>0.106208201048954</v>
       </c>
       <c r="E6" t="n">
-        <v>1.90648350187855</v>
+        <v>2.14618943486379</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.000295237688554051</v>
+        <v>0.0154935850975626</v>
       </c>
       <c r="H6" t="s">
         <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -2419,25 +2419,25 @@
         <v>-1.34903800414999</v>
       </c>
       <c r="C7" t="n">
-        <v>0.419042880366349</v>
+        <v>0.500708857594736</v>
       </c>
       <c r="D7" t="n">
-        <v>-2.57901244403367</v>
+        <v>-2.81871837701892</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.119063564266316</v>
+        <v>0.120642368718928</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0167036722763142</v>
+        <v>0.0917096570364839</v>
       </c>
       <c r="H7" t="s">
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
@@ -2448,25 +2448,25 @@
         <v>-1.31254760567531</v>
       </c>
       <c r="C8" t="n">
-        <v>0.452848906197681</v>
+        <v>0.534514883426069</v>
       </c>
       <c r="D8" t="n">
-        <v>-2.64174947462361</v>
+        <v>-2.88145540760885</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0166542632729858</v>
+        <v>0.256360196258229</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0487557977069047</v>
+        <v>0.182851296535574</v>
       </c>
       <c r="H8" t="s">
         <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
@@ -2477,19 +2477,19 @@
         <v>1.34611942528998</v>
       </c>
       <c r="C9" t="n">
-        <v>0.513969322148099</v>
+        <v>0.595635299376487</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.162483056092899</v>
+        <v>-0.402188989078142</v>
       </c>
       <c r="E9" t="n">
-        <v>2.85472190667286</v>
+        <v>3.0944278396581</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.114622251739836</v>
+        <v>0.309698410565498</v>
       </c>
       <c r="H9" t="s">
         <v>10</v>
@@ -2500,25 +2500,25 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="n">
         <v>1.12563245824976</v>
       </c>
       <c r="C10" t="n">
-        <v>0.521004365209251</v>
+        <v>0.602670342437638</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.403619277789666</v>
+        <v>-0.643325210774909</v>
       </c>
       <c r="E10" t="n">
-        <v>2.65488419428918</v>
+        <v>2.89459012727442</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.399536910593837</v>
+        <v>0.803375297133251</v>
       </c>
       <c r="H10" t="s">
         <v>10</v>
@@ -2529,19 +2529,19 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="n">
         <v>-0.409649207409245</v>
       </c>
       <c r="C11" t="n">
-        <v>0.469317262644103</v>
+        <v>0.550983239872491</v>
       </c>
       <c r="D11" t="n">
-        <v>-1.78718898745219</v>
+        <v>-2.02689492043743</v>
       </c>
       <c r="E11" t="n">
-        <v>0.967890572633699</v>
+        <v>1.20759650561894</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -2564,13 +2564,13 @@
         <v>0.0907686684785104</v>
       </c>
       <c r="C12" t="n">
-        <v>0.25191648859296</v>
+        <v>0.333582465821347</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.648656475038309</v>
+        <v>-0.888362408023552</v>
       </c>
       <c r="E12" t="n">
-        <v>0.830193811995329</v>
+        <v>1.06989974498057</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -2587,19 +2587,19 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="n">
         <v>-0.274703212183046</v>
       </c>
       <c r="C13" t="n">
-        <v>0.248855541894919</v>
+        <v>0.330521519123307</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.00514386657755</v>
+        <v>-1.24484979956279</v>
       </c>
       <c r="E13" t="n">
-        <v>0.455737442211455</v>
+        <v>0.695443375196698</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -2616,19 +2616,19 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B14" t="n">
         <v>0.00526298379007351</v>
       </c>
       <c r="C14" t="n">
-        <v>0.140270323689337</v>
+        <v>0.221936300917725</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.406458395800629</v>
+        <v>-0.646164328785873</v>
       </c>
       <c r="E14" t="n">
-        <v>0.416984363380776</v>
+        <v>0.65669029636602</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -2651,13 +2651,13 @@
         <v>-0.108883874006839</v>
       </c>
       <c r="C15" t="n">
-        <v>0.308788529427282</v>
+        <v>0.39045450665567</v>
       </c>
       <c r="D15" t="n">
-        <v>-1.01523980157393</v>
+        <v>-1.25494573455917</v>
       </c>
       <c r="E15" t="n">
-        <v>0.797472053560249</v>
+        <v>1.03717798654549</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -2680,13 +2680,13 @@
         <v>0.219364407734019</v>
       </c>
       <c r="C16" t="n">
-        <v>0.210859760649908</v>
+        <v>0.292525737878296</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.399551049730951</v>
+        <v>-0.639256982716194</v>
       </c>
       <c r="E16" t="n">
-        <v>0.838279865198988</v>
+        <v>1.07798579818423</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -2810,19 +2810,19 @@
         <v>-1.65084418948903</v>
       </c>
       <c r="C3" t="n">
-        <v>0.64428990763678</v>
+        <v>0.759335571046395</v>
       </c>
       <c r="D3" t="n">
-        <v>-3.52812865000751</v>
+        <v>-3.86334022729435</v>
       </c>
       <c r="E3" t="n">
-        <v>0.226440271029456</v>
+        <v>0.561651848316287</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.135187881455155</v>
+        <v>0.386104200571638</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
@@ -2839,19 +2839,19 @@
         <v>1.66884383726834</v>
       </c>
       <c r="C4" t="n">
-        <v>0.718294848081642</v>
+        <v>0.833340511491258</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.424070765911102</v>
+        <v>-0.759282343197933</v>
       </c>
       <c r="E4" t="n">
-        <v>3.76175844044779</v>
+        <v>4.09697001773462</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.262090964314637</v>
+        <v>0.587869605413677</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
@@ -2862,25 +2862,25 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.634087549662734</v>
+        <v>-0.673126139068271</v>
       </c>
       <c r="C5" t="n">
-        <v>0.283354815360677</v>
+        <v>0.524465414274835</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.45970593260591</v>
+        <v>-2.20127481969698</v>
       </c>
       <c r="E5" t="n">
-        <v>0.191530833280438</v>
+        <v>0.855022541560436</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.328054847887565</v>
+        <v>1</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
@@ -2891,25 +2891,25 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>1.65250752118857</v>
+        <v>0.204938049276485</v>
       </c>
       <c r="C6" t="n">
-        <v>0.912564435578408</v>
+        <v>0.457245117592772</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.00645549193216</v>
+        <v>-1.12734908378345</v>
       </c>
       <c r="E6" t="n">
-        <v>4.3114705343093</v>
+        <v>1.53722518233642</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.912154551276964</v>
+        <v>1</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
@@ -2920,19 +2920,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.673126139068271</v>
+        <v>0.699231034828448</v>
       </c>
       <c r="C7" t="n">
-        <v>0.409419750865219</v>
+        <v>0.676135390017139</v>
       </c>
       <c r="D7" t="n">
-        <v>-1.86606324241015</v>
+        <v>-1.27084244582174</v>
       </c>
       <c r="E7" t="n">
-        <v>0.519810964273604</v>
+        <v>2.66930451547864</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -2952,16 +2952,16 @@
         <v>21</v>
       </c>
       <c r="B8" t="n">
-        <v>0.204938049276485</v>
+        <v>0.656919424047354</v>
       </c>
       <c r="C8" t="n">
-        <v>0.342199454183156</v>
+        <v>0.693138519186517</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.792137506496622</v>
+        <v>-1.36269652155769</v>
       </c>
       <c r="E8" t="n">
-        <v>1.20201360504959</v>
+        <v>2.6765353696524</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -2978,19 +2978,19 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B9" t="n">
-        <v>0.699231034828448</v>
+        <v>0.00541284716531187</v>
       </c>
       <c r="C9" t="n">
-        <v>0.561089726607524</v>
+        <v>0.411426924205864</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.935630868534913</v>
+        <v>-1.19337260996466</v>
       </c>
       <c r="E9" t="n">
-        <v>2.33409293819181</v>
+        <v>1.20419830429529</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -3007,19 +3007,19 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>0.656919424047354</v>
+        <v>-0.978614048590889</v>
       </c>
       <c r="C10" t="n">
-        <v>0.578092855776901</v>
+        <v>0.710199352184258</v>
       </c>
       <c r="D10" t="n">
-        <v>-1.02748494427086</v>
+        <v>-3.04794059231416</v>
       </c>
       <c r="E10" t="n">
-        <v>2.34132379236557</v>
+        <v>1.09071249513238</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -3036,19 +3036,19 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" t="n">
-        <v>0.00541284716531187</v>
+        <v>-0.781037226566709</v>
       </c>
       <c r="C11" t="n">
-        <v>0.296381260796249</v>
+        <v>0.765835471520427</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.858161032677831</v>
+        <v>-3.01247219544977</v>
       </c>
       <c r="E11" t="n">
-        <v>0.868986727008455</v>
+        <v>1.45039774231635</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -3065,19 +3065,19 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.978614048590889</v>
+        <v>-0.142316177794834</v>
       </c>
       <c r="C12" t="n">
-        <v>0.595153688774643</v>
+        <v>0.456440982975699</v>
       </c>
       <c r="D12" t="n">
-        <v>-2.71272901502733</v>
+        <v>-1.47226028265752</v>
       </c>
       <c r="E12" t="n">
-        <v>0.755500917845551</v>
+        <v>1.18762792706785</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -3094,19 +3094,19 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.781037226566709</v>
+        <v>1.65250752118857</v>
       </c>
       <c r="C13" t="n">
-        <v>0.650789808110812</v>
+        <v>1.02761009898802</v>
       </c>
       <c r="D13" t="n">
-        <v>-2.67726061816293</v>
+        <v>-1.34166706921899</v>
       </c>
       <c r="E13" t="n">
-        <v>1.11518616502952</v>
+        <v>4.64668211159613</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -3123,19 +3123,19 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.142316177794834</v>
+        <v>-0.634087549662734</v>
       </c>
       <c r="C14" t="n">
-        <v>0.341395319566083</v>
+        <v>0.398400478770293</v>
       </c>
       <c r="D14" t="n">
-        <v>-1.13704870537069</v>
+        <v>-1.79491750989274</v>
       </c>
       <c r="E14" t="n">
-        <v>0.852416349781023</v>
+        <v>0.526742410567268</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -3158,13 +3158,13 @@
         <v>-0.399979368736203</v>
       </c>
       <c r="C15" t="n">
-        <v>0.29199046920467</v>
+        <v>0.407036132614286</v>
       </c>
       <c r="D15" t="n">
-        <v>-1.25075968356064</v>
+        <v>-1.58597126084747</v>
       </c>
       <c r="E15" t="n">
-        <v>0.450800946088237</v>
+        <v>0.786012523375067</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Change notations of EM algorithm.
</commit_message>
<xml_diff>
--- a/tables/Supplementary Table 1.xlsx
+++ b/tables/Supplementary Table 1.xlsx
@@ -1014,19 +1014,19 @@
         <v>6.25623454531064</v>
       </c>
       <c r="C5" t="n">
-        <v>0.957108005020814</v>
+        <v>0.523087230142417</v>
       </c>
       <c r="D5" t="n">
-        <v>3.46748376159302</v>
+        <v>4.73210151606007</v>
       </c>
       <c r="E5" t="n">
-        <v>9.04498532902826</v>
+        <v>7.78036757456121</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.000000000692252311891259</v>
+        <v>0.0000000000000000000000000000000631561162884799</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
@@ -1043,193 +1043,193 @@
         <v>-4.26076892184244</v>
       </c>
       <c r="C6" t="n">
-        <v>1.09110134329533</v>
+        <v>0.657080568416928</v>
       </c>
       <c r="D6" t="n">
-        <v>-7.43993962177198</v>
+        <v>-6.17532186730493</v>
       </c>
       <c r="E6" t="n">
-        <v>-1.0815982219129</v>
+        <v>-2.34621597637995</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.00103640783997099</v>
+        <v>0.000000000979984149253423</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" t="n">
-        <v>3.55358160279929</v>
+        <v>-1.90948397329009</v>
       </c>
       <c r="C7" t="n">
-        <v>1.08596539359687</v>
+        <v>0.327947613564495</v>
       </c>
       <c r="D7" t="n">
-        <v>0.389375654675779</v>
+        <v>-2.8650335659679</v>
       </c>
       <c r="E7" t="n">
-        <v>6.7177875509228</v>
+        <v>-0.953934380612283</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0117352722684026</v>
+        <v>0.0000000637607134769436</v>
       </c>
       <c r="H7" t="s">
         <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>3.06690070843383</v>
+        <v>3.55358160279929</v>
       </c>
       <c r="C8" t="n">
-        <v>1.05340860543981</v>
+        <v>0.651944618718474</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.00244366919600925</v>
+        <v>1.65399340914283</v>
       </c>
       <c r="E8" t="n">
-        <v>6.13624508606367</v>
+        <v>5.45316979645576</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0395786076941127</v>
+        <v>0.00000055176253185185</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.90948397329009</v>
+        <v>3.06690070843383</v>
       </c>
       <c r="C9" t="n">
-        <v>0.761968388442892</v>
+        <v>0.61938783056141</v>
       </c>
       <c r="D9" t="n">
-        <v>-4.12965132043495</v>
+        <v>1.26217408527104</v>
       </c>
       <c r="E9" t="n">
-        <v>0.310683373854766</v>
+        <v>4.87162733159662</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.134320573116715</v>
+        <v>0.00000810067278349778</v>
       </c>
       <c r="H9" t="s">
         <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B10" t="n">
-        <v>0.10610149948576</v>
+        <v>1.17466221039992</v>
       </c>
       <c r="C10" t="n">
-        <v>0.703997381356196</v>
+        <v>0.279612295989963</v>
       </c>
       <c r="D10" t="n">
-        <v>-1.94515419861024</v>
+        <v>0.359948504644077</v>
       </c>
       <c r="E10" t="n">
-        <v>2.15735719758176</v>
+        <v>1.98937591615577</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>0.000292261862215732</v>
       </c>
       <c r="H10" t="s">
         <v>26</v>
       </c>
       <c r="I10" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.62157578854071</v>
+        <v>-0.747832996345051</v>
       </c>
       <c r="C11" t="n">
-        <v>0.653567945591162</v>
+        <v>0.222236147680543</v>
       </c>
       <c r="D11" t="n">
-        <v>-2.52589391242938</v>
+        <v>-1.39536830872709</v>
       </c>
       <c r="E11" t="n">
-        <v>1.28274233534796</v>
+        <v>-0.100297683963016</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>0.00841865471512599</v>
       </c>
       <c r="H11" t="s">
         <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B12" t="n">
-        <v>0.870330512046186</v>
+        <v>-0.62157578854071</v>
       </c>
       <c r="C12" t="n">
-        <v>0.916654644119761</v>
+        <v>0.219547170712765</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.80055024934896</v>
+        <v>-1.26127615796233</v>
       </c>
       <c r="E12" t="n">
-        <v>3.54121127344133</v>
+        <v>0.0181245808809136</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>0.0510155612256206</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
@@ -1240,25 +1240,25 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>1.17466221039992</v>
+        <v>0.870330512046186</v>
       </c>
       <c r="C13" t="n">
-        <v>0.71363307086836</v>
+        <v>0.482633869241364</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.904669249822971</v>
+        <v>-0.535932494881909</v>
       </c>
       <c r="E13" t="n">
-        <v>3.25399367062282</v>
+        <v>2.27659351897428</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>0.784763487986671</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
@@ -1269,19 +1269,19 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.0842444756762468</v>
+        <v>0.10610149948576</v>
       </c>
       <c r="C14" t="n">
-        <v>0.669521340289233</v>
+        <v>0.269976606477799</v>
       </c>
       <c r="D14" t="n">
-        <v>-2.03504642556346</v>
+        <v>-0.680536444143195</v>
       </c>
       <c r="E14" t="n">
-        <v>1.86655747421097</v>
+        <v>0.892739443114715</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -1298,19 +1298,19 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.747832996345051</v>
+        <v>-0.0842444756762468</v>
       </c>
       <c r="C15" t="n">
-        <v>0.656256922558941</v>
+        <v>0.235500565410835</v>
       </c>
       <c r="D15" t="n">
-        <v>-2.65998606319414</v>
+        <v>-0.770428671096416</v>
       </c>
       <c r="E15" t="n">
-        <v>1.16432007050403</v>
+        <v>0.601939719743922</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -1434,19 +1434,19 @@
         <v>4.1685101478655</v>
       </c>
       <c r="C4" t="n">
-        <v>0.540782286471597</v>
+        <v>0.525773545331223</v>
       </c>
       <c r="D4" t="n">
-        <v>2.60537269700204</v>
+        <v>2.64875563677972</v>
       </c>
       <c r="E4" t="n">
-        <v>5.73164759872896</v>
+        <v>5.68826465895128</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.000000000000140259178742054</v>
+        <v>0.0000000000000244308815932119</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
@@ -1463,19 +1463,19 @@
         <v>2.10996832913156</v>
       </c>
       <c r="C5" t="n">
-        <v>0.513384241125952</v>
+        <v>0.498375499985579</v>
       </c>
       <c r="D5" t="n">
-        <v>0.626025245080044</v>
+        <v>0.669408184857722</v>
       </c>
       <c r="E5" t="n">
-        <v>3.59391141318308</v>
+        <v>3.5505284734054</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0004353752159312</v>
+        <v>0.000252874398556954</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -1492,25 +1492,25 @@
         <v>1.83129046738175</v>
       </c>
       <c r="C6" t="n">
-        <v>0.552476647809693</v>
+        <v>0.53746790666932</v>
       </c>
       <c r="D6" t="n">
-        <v>0.234350329875614</v>
+        <v>0.277733269653293</v>
       </c>
       <c r="E6" t="n">
-        <v>3.42823060488789</v>
+        <v>3.38484766511021</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0100918210950258</v>
+        <v>0.0072181643495806</v>
       </c>
       <c r="H6" t="s">
         <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
@@ -1521,19 +1521,19 @@
         <v>1.49086520407092</v>
       </c>
       <c r="C7" t="n">
-        <v>0.607554539446084</v>
+        <v>0.59254579830571</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.265278215948726</v>
+        <v>-0.221895276171048</v>
       </c>
       <c r="E7" t="n">
-        <v>3.24700862409057</v>
+        <v>3.20362568431289</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.155457065548552</v>
+        <v>0.130552213089341</v>
       </c>
       <c r="H7" t="s">
         <v>10</v>
@@ -1550,13 +1550,13 @@
         <v>-0.244262374583913</v>
       </c>
       <c r="C8" t="n">
-        <v>0.67610045151486</v>
+        <v>0.661091710374487</v>
       </c>
       <c r="D8" t="n">
-        <v>-2.19853854587652</v>
+        <v>-2.15515560609884</v>
       </c>
       <c r="E8" t="n">
-        <v>1.71001379670869</v>
+        <v>1.66663085693102</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -1579,13 +1579,13 @@
         <v>0.392631542156252</v>
       </c>
       <c r="C9" t="n">
-        <v>0.388206229771094</v>
+        <v>0.373197488630721</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.729483052929649</v>
+        <v>-0.686100113151971</v>
       </c>
       <c r="E9" t="n">
-        <v>1.51474613724215</v>
+        <v>1.47136319746448</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -1608,13 +1608,13 @@
         <v>-0.0916681019861905</v>
       </c>
       <c r="C10" t="n">
-        <v>0.285175507969297</v>
+        <v>0.270166766828923</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.915971204597582</v>
+        <v>-0.872588264819903</v>
       </c>
       <c r="E10" t="n">
-        <v>0.732635000625201</v>
+        <v>0.689252060847522</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -1637,13 +1637,13 @@
         <v>-0.0367122110826159</v>
       </c>
       <c r="C11" t="n">
-        <v>0.473744924138665</v>
+        <v>0.458736182998291</v>
       </c>
       <c r="D11" t="n">
-        <v>-1.40607739112446</v>
+        <v>-1.36269445134678</v>
       </c>
       <c r="E11" t="n">
-        <v>1.33265296895923</v>
+        <v>1.28927002918155</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -1666,13 +1666,13 @@
         <v>-0.130887533638454</v>
       </c>
       <c r="C12" t="n">
-        <v>0.598400441691161</v>
+        <v>0.583391700550788</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.8605709282698</v>
+        <v>-1.81718798849212</v>
       </c>
       <c r="E12" t="n">
-        <v>1.59879586099289</v>
+        <v>1.55541292121521</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -1695,13 +1695,13 @@
         <v>0.058655285470948</v>
       </c>
       <c r="C13" t="n">
-        <v>0.337418831844216</v>
+        <v>0.322410090703843</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.916657748769861</v>
+        <v>-0.873274808992183</v>
       </c>
       <c r="E13" t="n">
-        <v>1.03396831971176</v>
+        <v>0.990585379934079</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -1724,13 +1724,13 @@
         <v>-0.819900657033559</v>
       </c>
       <c r="C14" t="n">
-        <v>0.821653548025072</v>
+        <v>0.806644806884698</v>
       </c>
       <c r="D14" t="n">
-        <v>-3.19489973648341</v>
+        <v>-3.15151679670573</v>
       </c>
       <c r="E14" t="n">
-        <v>1.5550984224163</v>
+        <v>1.51171548263862</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -1877,25 +1877,25 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B4" t="n">
-        <v>-2.28116311114461</v>
+        <v>3.88050543051919</v>
       </c>
       <c r="C4" t="n">
-        <v>0.351898043856357</v>
+        <v>0.76171110714712</v>
       </c>
       <c r="D4" t="n">
-        <v>-3.30649770289925</v>
+        <v>1.66108773065704</v>
       </c>
       <c r="E4" t="n">
-        <v>-1.25582851938997</v>
+        <v>6.09992313038134</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00000000108290656147483</v>
+        <v>0.00000419687881524945</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
@@ -1906,25 +1906,25 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B5" t="n">
-        <v>3.88050543051919</v>
+        <v>-2.28116311114461</v>
       </c>
       <c r="C5" t="n">
-        <v>0.635089430400732</v>
+        <v>0.478519720602745</v>
       </c>
       <c r="D5" t="n">
-        <v>2.03002864266461</v>
+        <v>-3.67543861490682</v>
       </c>
       <c r="E5" t="n">
-        <v>5.73098221837376</v>
+        <v>-0.886887607382393</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0000000119428849615354</v>
+        <v>0.0000224248546027849</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
@@ -1941,19 +1941,19 @@
         <v>-2.87261124480962</v>
       </c>
       <c r="C6" t="n">
-        <v>0.478242093245063</v>
+        <v>0.604863769991451</v>
       </c>
       <c r="D6" t="n">
-        <v>-4.26607781843306</v>
+        <v>-4.63501873044063</v>
       </c>
       <c r="E6" t="n">
-        <v>-1.47914467118617</v>
+        <v>-1.1102037591786</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0000000227338268801947</v>
+        <v>0.0000245083049393418</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
@@ -1970,19 +1970,19 @@
         <v>-4.27886174538928</v>
       </c>
       <c r="C7" t="n">
-        <v>0.775253628039198</v>
+        <v>0.901875304785586</v>
       </c>
       <c r="D7" t="n">
-        <v>-6.53773864479127</v>
+        <v>-6.90667955679884</v>
       </c>
       <c r="E7" t="n">
-        <v>-2.01998484598729</v>
+        <v>-1.65104393397971</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.000000408410077974224</v>
+        <v>0.0000250944052996328</v>
       </c>
       <c r="H7" t="s">
         <v>26</v>
@@ -1999,112 +1999,112 @@
         <v>-2.02435170757185</v>
       </c>
       <c r="C8" t="n">
-        <v>0.391845637186683</v>
+        <v>0.518467313933071</v>
       </c>
       <c r="D8" t="n">
-        <v>-3.16608265336718</v>
+        <v>-3.53502356537475</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.882620761776526</v>
+        <v>-0.513679849768952</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.00000286686174126159</v>
+        <v>0.00113308012398904</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.7448313110769</v>
+        <v>2.68862406807983</v>
       </c>
       <c r="C9" t="n">
-        <v>0.419913660508586</v>
+        <v>0.821113025597041</v>
       </c>
       <c r="D9" t="n">
-        <v>-2.96834479512888</v>
+        <v>0.296125435070596</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.521317827024919</v>
+        <v>5.08112270108906</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.000389979098703508</v>
+        <v>0.0127079498546506</v>
       </c>
       <c r="H9" t="s">
         <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B10" t="n">
-        <v>-2.10047574233186</v>
+        <v>-1.7448313110769</v>
       </c>
       <c r="C10" t="n">
-        <v>0.534663915095059</v>
+        <v>0.546535337254974</v>
       </c>
       <c r="D10" t="n">
-        <v>-3.65834006320801</v>
+        <v>-3.33728570713645</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.542611421455714</v>
+        <v>-0.152376915017345</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.00102534103083569</v>
+        <v>0.0169237840330592</v>
       </c>
       <c r="H10" t="s">
         <v>26</v>
       </c>
       <c r="I10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B11" t="n">
-        <v>2.68862406807983</v>
+        <v>-2.10047574233186</v>
       </c>
       <c r="C11" t="n">
-        <v>0.694491348850653</v>
+        <v>0.661285591841447</v>
       </c>
       <c r="D11" t="n">
-        <v>0.66506634707817</v>
+        <v>-4.02728097521559</v>
       </c>
       <c r="E11" t="n">
-        <v>4.71218178908149</v>
+        <v>-0.173670509448141</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00129877278194209</v>
+        <v>0.017896790543035</v>
       </c>
       <c r="H11" t="s">
         <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12">
@@ -2115,19 +2115,19 @@
         <v>-1.1043314014521</v>
       </c>
       <c r="C12" t="n">
-        <v>0.416575541752966</v>
+        <v>0.543197218499354</v>
       </c>
       <c r="D12" t="n">
-        <v>-2.3181185210321</v>
+        <v>-2.68705943303967</v>
       </c>
       <c r="E12" t="n">
-        <v>0.109455718127904</v>
+        <v>0.478396630135478</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0963117009539047</v>
+        <v>0.50460470737746</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
@@ -2144,13 +2144,13 @@
         <v>0.737240752555557</v>
       </c>
       <c r="C13" t="n">
-        <v>0.785573041376803</v>
+        <v>0.912194718123191</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.55170409307798</v>
+        <v>-1.92064500508556</v>
       </c>
       <c r="E13" t="n">
-        <v>3.0261855981891</v>
+        <v>3.39512651019667</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -2173,13 +2173,13 @@
         <v>0.186861675188612</v>
       </c>
       <c r="C14" t="n">
-        <v>0.733385928014918</v>
+        <v>0.860007604761306</v>
       </c>
       <c r="D14" t="n">
-        <v>-1.95002420476451</v>
+        <v>-2.31896511677208</v>
       </c>
       <c r="E14" t="n">
-        <v>2.32374755514173</v>
+        <v>2.69268846714931</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -2202,13 +2202,13 @@
         <v>-0.337196087243825</v>
       </c>
       <c r="C15" t="n">
-        <v>0.519900376901564</v>
+        <v>0.646522053647952</v>
       </c>
       <c r="D15" t="n">
-        <v>-1.85204349833385</v>
+        <v>-2.22098441034143</v>
       </c>
       <c r="E15" t="n">
-        <v>1.1776513238462</v>
+        <v>1.54659223585378</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -2332,19 +2332,19 @@
         <v>-2.97705281260192</v>
       </c>
       <c r="C4" t="n">
-        <v>0.645069794567981</v>
+        <v>0.65887845702337</v>
       </c>
       <c r="D4" t="n">
-        <v>-4.8704613309998</v>
+        <v>-4.91099250970462</v>
       </c>
       <c r="E4" t="n">
-        <v>-1.08364429420403</v>
+        <v>-1.04311311549921</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.000051081145091242</v>
+        <v>0.000081015001416609</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
@@ -2361,19 +2361,19 @@
         <v>-2.36911056677888</v>
       </c>
       <c r="C5" t="n">
-        <v>0.539393707141817</v>
+        <v>0.553202369597206</v>
       </c>
       <c r="D5" t="n">
-        <v>-3.95233868949158</v>
+        <v>-3.9928698681964</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.785882444066181</v>
+        <v>-0.745351265361361</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00014589023435706</v>
+        <v>0.000240204857568503</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -2390,19 +2390,19 @@
         <v>1.12619881795637</v>
       </c>
       <c r="C6" t="n">
-        <v>0.34750299859561</v>
+        <v>0.361311661051</v>
       </c>
       <c r="D6" t="n">
-        <v>0.106208201048954</v>
+        <v>0.0656770223441343</v>
       </c>
       <c r="E6" t="n">
-        <v>2.14618943486379</v>
+        <v>2.18672061356861</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0154935850975626</v>
+        <v>0.0237533516665213</v>
       </c>
       <c r="H6" t="s">
         <v>10</v>
@@ -2419,19 +2419,19 @@
         <v>-1.34903800414999</v>
       </c>
       <c r="C7" t="n">
-        <v>0.500708857594736</v>
+        <v>0.514517520050126</v>
       </c>
       <c r="D7" t="n">
-        <v>-2.81871837701892</v>
+        <v>-2.85924955572374</v>
       </c>
       <c r="E7" t="n">
-        <v>0.120642368718928</v>
+        <v>0.161173547423747</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0917096570364839</v>
+        <v>0.113657516207731</v>
       </c>
       <c r="H7" t="s">
         <v>10</v>
@@ -2448,19 +2448,19 @@
         <v>-1.31254760567531</v>
       </c>
       <c r="C8" t="n">
-        <v>0.534514883426069</v>
+        <v>0.548323545881458</v>
       </c>
       <c r="D8" t="n">
-        <v>-2.88145540760885</v>
+        <v>-2.92198658631367</v>
       </c>
       <c r="E8" t="n">
-        <v>0.256360196258229</v>
+        <v>0.296891374963048</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.182851296535574</v>
+        <v>0.216804480509727</v>
       </c>
       <c r="H8" t="s">
         <v>10</v>
@@ -2477,19 +2477,19 @@
         <v>1.34611942528998</v>
       </c>
       <c r="C9" t="n">
-        <v>0.595635299376487</v>
+        <v>0.609443961831876</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.402188989078142</v>
+        <v>-0.442720167782961</v>
       </c>
       <c r="E9" t="n">
-        <v>3.0944278396581</v>
+        <v>3.13495901836292</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.309698410565498</v>
+        <v>0.35348149374962</v>
       </c>
       <c r="H9" t="s">
         <v>10</v>
@@ -2506,19 +2506,19 @@
         <v>1.12563245824976</v>
       </c>
       <c r="C10" t="n">
-        <v>0.602670342437638</v>
+        <v>0.616479004893028</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.643325210774909</v>
+        <v>-0.683856389479728</v>
       </c>
       <c r="E10" t="n">
-        <v>2.89459012727442</v>
+        <v>2.93512130597924</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.803375297133251</v>
+        <v>0.882238301715663</v>
       </c>
       <c r="H10" t="s">
         <v>10</v>
@@ -2535,13 +2535,13 @@
         <v>-0.409649207409245</v>
       </c>
       <c r="C11" t="n">
-        <v>0.550983239872491</v>
+        <v>0.56479190232788</v>
       </c>
       <c r="D11" t="n">
-        <v>-2.02689492043743</v>
+        <v>-2.06742609914225</v>
       </c>
       <c r="E11" t="n">
-        <v>1.20759650561894</v>
+        <v>1.24812768432376</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -2564,13 +2564,13 @@
         <v>0.0907686684785104</v>
       </c>
       <c r="C12" t="n">
-        <v>0.333582465821347</v>
+        <v>0.347391128276737</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.888362408023552</v>
+        <v>-0.928893586728371</v>
       </c>
       <c r="E12" t="n">
-        <v>1.06989974498057</v>
+        <v>1.11043092368539</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -2593,13 +2593,13 @@
         <v>-0.274703212183046</v>
       </c>
       <c r="C13" t="n">
-        <v>0.330521519123307</v>
+        <v>0.344330181578696</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.24484979956279</v>
+        <v>-1.28538097826761</v>
       </c>
       <c r="E13" t="n">
-        <v>0.695443375196698</v>
+        <v>0.735974553901517</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -2622,13 +2622,13 @@
         <v>0.00526298379007351</v>
       </c>
       <c r="C14" t="n">
-        <v>0.221936300917725</v>
+        <v>0.235744963373115</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.646164328785873</v>
+        <v>-0.686695507490692</v>
       </c>
       <c r="E14" t="n">
-        <v>0.65669029636602</v>
+        <v>0.697221475070839</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -2651,13 +2651,13 @@
         <v>-0.108883874006839</v>
       </c>
       <c r="C15" t="n">
-        <v>0.39045450665567</v>
+        <v>0.40426316911106</v>
       </c>
       <c r="D15" t="n">
-        <v>-1.25494573455917</v>
+        <v>-1.29547691326399</v>
       </c>
       <c r="E15" t="n">
-        <v>1.03717798654549</v>
+        <v>1.07770916525031</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -2680,13 +2680,13 @@
         <v>0.219364407734019</v>
       </c>
       <c r="C16" t="n">
-        <v>0.292525737878296</v>
+        <v>0.306334400333686</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.639256982716194</v>
+        <v>-0.679788161421014</v>
       </c>
       <c r="E16" t="n">
-        <v>1.07798579818423</v>
+        <v>1.11851697688905</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -2810,19 +2810,19 @@
         <v>-1.65084418948903</v>
       </c>
       <c r="C3" t="n">
-        <v>0.759335571046395</v>
+        <v>0.814155925898332</v>
       </c>
       <c r="D3" t="n">
-        <v>-3.86334022729435</v>
+        <v>-4.02307173800686</v>
       </c>
       <c r="E3" t="n">
-        <v>0.561651848316287</v>
+        <v>0.7213833590288</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.386104200571638</v>
+        <v>0.5537136409522</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
@@ -2839,19 +2839,19 @@
         <v>1.66884383726834</v>
       </c>
       <c r="C4" t="n">
-        <v>0.833340511491258</v>
+        <v>0.888160866343194</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.759282343197933</v>
+        <v>-0.919013853910447</v>
       </c>
       <c r="E4" t="n">
-        <v>4.09697001773462</v>
+        <v>4.25670152844713</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.587869605413677</v>
+        <v>0.783199258548616</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
@@ -2868,13 +2868,13 @@
         <v>-0.673126139068271</v>
       </c>
       <c r="C5" t="n">
-        <v>0.524465414274835</v>
+        <v>0.579285769126771</v>
       </c>
       <c r="D5" t="n">
-        <v>-2.20127481969698</v>
+        <v>-2.36100633040949</v>
       </c>
       <c r="E5" t="n">
-        <v>0.855022541560436</v>
+        <v>1.01475405227295</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -2897,13 +2897,13 @@
         <v>0.204938049276485</v>
       </c>
       <c r="C6" t="n">
-        <v>0.457245117592772</v>
+        <v>0.512065472444708</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.12734908378345</v>
+        <v>-1.28708059449597</v>
       </c>
       <c r="E6" t="n">
-        <v>1.53722518233642</v>
+        <v>1.69695669304894</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -2926,13 +2926,13 @@
         <v>0.699231034828448</v>
       </c>
       <c r="C7" t="n">
-        <v>0.676135390017139</v>
+        <v>0.730955744869076</v>
       </c>
       <c r="D7" t="n">
-        <v>-1.27084244582174</v>
+        <v>-1.43057395653426</v>
       </c>
       <c r="E7" t="n">
-        <v>2.66930451547864</v>
+        <v>2.82903602619115</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -2955,13 +2955,13 @@
         <v>0.656919424047354</v>
       </c>
       <c r="C8" t="n">
-        <v>0.693138519186517</v>
+        <v>0.747958874038453</v>
       </c>
       <c r="D8" t="n">
-        <v>-1.36269652155769</v>
+        <v>-1.5224280322702</v>
       </c>
       <c r="E8" t="n">
-        <v>2.6765353696524</v>
+        <v>2.83626688036491</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -2984,13 +2984,13 @@
         <v>0.00541284716531187</v>
       </c>
       <c r="C9" t="n">
-        <v>0.411426924205864</v>
+        <v>0.4662472790578</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.19337260996466</v>
+        <v>-1.35310412067718</v>
       </c>
       <c r="E9" t="n">
-        <v>1.20419830429529</v>
+        <v>1.3639298150078</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -3013,13 +3013,13 @@
         <v>-0.978614048590889</v>
       </c>
       <c r="C10" t="n">
-        <v>0.710199352184258</v>
+        <v>0.765019707036194</v>
       </c>
       <c r="D10" t="n">
-        <v>-3.04794059231416</v>
+        <v>-3.20767210302667</v>
       </c>
       <c r="E10" t="n">
-        <v>1.09071249513238</v>
+        <v>1.2504440058449</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -3042,13 +3042,13 @@
         <v>-0.781037226566709</v>
       </c>
       <c r="C11" t="n">
-        <v>0.765835471520427</v>
+        <v>0.820655826372363</v>
       </c>
       <c r="D11" t="n">
-        <v>-3.01247219544977</v>
+        <v>-3.17220370616228</v>
       </c>
       <c r="E11" t="n">
-        <v>1.45039774231635</v>
+        <v>1.61012925302886</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -3071,13 +3071,13 @@
         <v>-0.142316177794834</v>
       </c>
       <c r="C12" t="n">
-        <v>0.456440982975699</v>
+        <v>0.511261337827635</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.47226028265752</v>
+        <v>-1.63199179337004</v>
       </c>
       <c r="E12" t="n">
-        <v>1.18762792706785</v>
+        <v>1.34735943778037</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -3100,13 +3100,13 @@
         <v>1.65250752118857</v>
       </c>
       <c r="C13" t="n">
-        <v>1.02761009898802</v>
+        <v>1.08243045383996</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.34166706921899</v>
+        <v>-1.5013985799315</v>
       </c>
       <c r="E13" t="n">
-        <v>4.64668211159613</v>
+        <v>4.80641362230864</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -3129,13 +3129,13 @@
         <v>-0.634087549662734</v>
       </c>
       <c r="C14" t="n">
-        <v>0.398400478770293</v>
+        <v>0.453220833622229</v>
       </c>
       <c r="D14" t="n">
-        <v>-1.79491750989274</v>
+        <v>-1.95464902060525</v>
       </c>
       <c r="E14" t="n">
-        <v>0.526742410567268</v>
+        <v>0.686473921279782</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -3158,13 +3158,13 @@
         <v>-0.399979368736203</v>
       </c>
       <c r="C15" t="n">
-        <v>0.407036132614286</v>
+        <v>0.461856487466222</v>
       </c>
       <c r="D15" t="n">
-        <v>-1.58597126084747</v>
+        <v>-1.74570277155999</v>
       </c>
       <c r="E15" t="n">
-        <v>0.786012523375067</v>
+        <v>0.945744034087581</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Change the variance estimator of delta.
</commit_message>
<xml_diff>
--- a/tables/Supplementary Table 1.xlsx
+++ b/tables/Supplementary Table 1.xlsx
@@ -1014,19 +1014,19 @@
         <v>6.25623454531064</v>
       </c>
       <c r="C5" t="n">
-        <v>0.523087230142417</v>
+        <v>0.957108005020814</v>
       </c>
       <c r="D5" t="n">
-        <v>4.73210151606007</v>
+        <v>3.46748376159302</v>
       </c>
       <c r="E5" t="n">
-        <v>7.78036757456121</v>
+        <v>9.04498532902826</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0000000000000000000000000000000631561162884799</v>
+        <v>0.000000000692252311891259</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
@@ -1043,193 +1043,193 @@
         <v>-4.26076892184244</v>
       </c>
       <c r="C6" t="n">
-        <v>0.657080568416928</v>
+        <v>1.09110134329533</v>
       </c>
       <c r="D6" t="n">
-        <v>-6.17532186730493</v>
+        <v>-7.43993962177198</v>
       </c>
       <c r="E6" t="n">
-        <v>-2.34621597637995</v>
+        <v>-1.0815982219129</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.000000000979984149253423</v>
+        <v>0.00103640783997099</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.90948397329009</v>
+        <v>3.55358160279929</v>
       </c>
       <c r="C7" t="n">
-        <v>0.327947613564495</v>
+        <v>1.08596539359687</v>
       </c>
       <c r="D7" t="n">
-        <v>-2.8650335659679</v>
+        <v>0.389375654675779</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.953934380612283</v>
+        <v>6.7177875509228</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0000000637607134769436</v>
+        <v>0.0117352722684026</v>
       </c>
       <c r="H7" t="s">
         <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B8" t="n">
-        <v>3.55358160279929</v>
+        <v>3.06690070843383</v>
       </c>
       <c r="C8" t="n">
-        <v>0.651944618718474</v>
+        <v>1.05340860543981</v>
       </c>
       <c r="D8" t="n">
-        <v>1.65399340914283</v>
+        <v>-0.00244366919600925</v>
       </c>
       <c r="E8" t="n">
-        <v>5.45316979645576</v>
+        <v>6.13624508606367</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.00000055176253185185</v>
+        <v>0.0395786076941127</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" t="n">
-        <v>3.06690070843383</v>
+        <v>-1.90948397329009</v>
       </c>
       <c r="C9" t="n">
-        <v>0.61938783056141</v>
+        <v>0.761968388442892</v>
       </c>
       <c r="D9" t="n">
-        <v>1.26217408527104</v>
+        <v>-4.12965132043495</v>
       </c>
       <c r="E9" t="n">
-        <v>4.87162733159662</v>
+        <v>0.310683373854766</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.00000810067278349778</v>
+        <v>0.134320573116715</v>
       </c>
       <c r="H9" t="s">
         <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" t="n">
-        <v>1.17466221039992</v>
+        <v>0.10610149948576</v>
       </c>
       <c r="C10" t="n">
-        <v>0.279612295989963</v>
+        <v>0.703997381356196</v>
       </c>
       <c r="D10" t="n">
-        <v>0.359948504644077</v>
+        <v>-1.94515419861024</v>
       </c>
       <c r="E10" t="n">
-        <v>1.98937591615577</v>
+        <v>2.15735719758176</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.000292261862215732</v>
+        <v>1</v>
       </c>
       <c r="H10" t="s">
         <v>26</v>
       </c>
       <c r="I10" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.747832996345051</v>
+        <v>-0.62157578854071</v>
       </c>
       <c r="C11" t="n">
-        <v>0.222236147680543</v>
+        <v>0.653567945591162</v>
       </c>
       <c r="D11" t="n">
-        <v>-1.39536830872709</v>
+        <v>-2.52589391242938</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.100297683963016</v>
+        <v>1.28274233534796</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00841865471512599</v>
+        <v>1</v>
       </c>
       <c r="H11" t="s">
         <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.62157578854071</v>
+        <v>0.870330512046186</v>
       </c>
       <c r="C12" t="n">
-        <v>0.219547170712765</v>
+        <v>0.916654644119761</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.26127615796233</v>
+        <v>-1.80055024934896</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0181245808809136</v>
+        <v>3.54121127344133</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0510155612256206</v>
+        <v>1</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
@@ -1240,25 +1240,25 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B13" t="n">
-        <v>0.870330512046186</v>
+        <v>1.17466221039992</v>
       </c>
       <c r="C13" t="n">
-        <v>0.482633869241364</v>
+        <v>0.71363307086836</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.535932494881909</v>
+        <v>-0.904669249822971</v>
       </c>
       <c r="E13" t="n">
-        <v>2.27659351897428</v>
+        <v>3.25399367062282</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0.784763487986671</v>
+        <v>1</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
@@ -1269,19 +1269,19 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>0.10610149948576</v>
+        <v>-0.0842444756762468</v>
       </c>
       <c r="C14" t="n">
-        <v>0.269976606477799</v>
+        <v>0.669521340289233</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.680536444143195</v>
+        <v>-2.03504642556346</v>
       </c>
       <c r="E14" t="n">
-        <v>0.892739443114715</v>
+        <v>1.86655747421097</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -1298,19 +1298,19 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.0842444756762468</v>
+        <v>-0.747832996345051</v>
       </c>
       <c r="C15" t="n">
-        <v>0.235500565410835</v>
+        <v>0.656256922558941</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.770428671096416</v>
+        <v>-2.65998606319414</v>
       </c>
       <c r="E15" t="n">
-        <v>0.601939719743922</v>
+        <v>1.16432007050403</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -1434,19 +1434,19 @@
         <v>4.1685101478655</v>
       </c>
       <c r="C4" t="n">
-        <v>0.525773545331223</v>
+        <v>0.540782286471597</v>
       </c>
       <c r="D4" t="n">
-        <v>2.64875563677972</v>
+        <v>2.60537269700204</v>
       </c>
       <c r="E4" t="n">
-        <v>5.68826465895128</v>
+        <v>5.73164759872896</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0000000000000244308815932119</v>
+        <v>0.000000000000140259178742054</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
@@ -1463,19 +1463,19 @@
         <v>2.10996832913156</v>
       </c>
       <c r="C5" t="n">
-        <v>0.498375499985579</v>
+        <v>0.513384241125952</v>
       </c>
       <c r="D5" t="n">
-        <v>0.669408184857722</v>
+        <v>0.626025245080044</v>
       </c>
       <c r="E5" t="n">
-        <v>3.5505284734054</v>
+        <v>3.59391141318308</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.000252874398556954</v>
+        <v>0.0004353752159312</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -1492,25 +1492,25 @@
         <v>1.83129046738175</v>
       </c>
       <c r="C6" t="n">
-        <v>0.53746790666932</v>
+        <v>0.552476647809693</v>
       </c>
       <c r="D6" t="n">
-        <v>0.277733269653293</v>
+        <v>0.234350329875614</v>
       </c>
       <c r="E6" t="n">
-        <v>3.38484766511021</v>
+        <v>3.42823060488789</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0072181643495806</v>
+        <v>0.0100918210950258</v>
       </c>
       <c r="H6" t="s">
         <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -1521,19 +1521,19 @@
         <v>1.49086520407092</v>
       </c>
       <c r="C7" t="n">
-        <v>0.59254579830571</v>
+        <v>0.607554539446084</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.221895276171048</v>
+        <v>-0.265278215948726</v>
       </c>
       <c r="E7" t="n">
-        <v>3.20362568431289</v>
+        <v>3.24700862409057</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.130552213089341</v>
+        <v>0.155457065548552</v>
       </c>
       <c r="H7" t="s">
         <v>10</v>
@@ -1550,13 +1550,13 @@
         <v>-0.244262374583913</v>
       </c>
       <c r="C8" t="n">
-        <v>0.661091710374487</v>
+        <v>0.67610045151486</v>
       </c>
       <c r="D8" t="n">
-        <v>-2.15515560609884</v>
+        <v>-2.19853854587652</v>
       </c>
       <c r="E8" t="n">
-        <v>1.66663085693102</v>
+        <v>1.71001379670869</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -1579,13 +1579,13 @@
         <v>0.392631542156252</v>
       </c>
       <c r="C9" t="n">
-        <v>0.373197488630721</v>
+        <v>0.388206229771094</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.686100113151971</v>
+        <v>-0.729483052929649</v>
       </c>
       <c r="E9" t="n">
-        <v>1.47136319746448</v>
+        <v>1.51474613724215</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -1608,13 +1608,13 @@
         <v>-0.0916681019861905</v>
       </c>
       <c r="C10" t="n">
-        <v>0.270166766828923</v>
+        <v>0.285175507969297</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.872588264819903</v>
+        <v>-0.915971204597582</v>
       </c>
       <c r="E10" t="n">
-        <v>0.689252060847522</v>
+        <v>0.732635000625201</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -1637,13 +1637,13 @@
         <v>-0.0367122110826159</v>
       </c>
       <c r="C11" t="n">
-        <v>0.458736182998291</v>
+        <v>0.473744924138665</v>
       </c>
       <c r="D11" t="n">
-        <v>-1.36269445134678</v>
+        <v>-1.40607739112446</v>
       </c>
       <c r="E11" t="n">
-        <v>1.28927002918155</v>
+        <v>1.33265296895923</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -1666,13 +1666,13 @@
         <v>-0.130887533638454</v>
       </c>
       <c r="C12" t="n">
-        <v>0.583391700550788</v>
+        <v>0.598400441691161</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.81718798849212</v>
+        <v>-1.8605709282698</v>
       </c>
       <c r="E12" t="n">
-        <v>1.55541292121521</v>
+        <v>1.59879586099289</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -1695,13 +1695,13 @@
         <v>0.058655285470948</v>
       </c>
       <c r="C13" t="n">
-        <v>0.322410090703843</v>
+        <v>0.337418831844216</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.873274808992183</v>
+        <v>-0.916657748769861</v>
       </c>
       <c r="E13" t="n">
-        <v>0.990585379934079</v>
+        <v>1.03396831971176</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -1724,13 +1724,13 @@
         <v>-0.819900657033559</v>
       </c>
       <c r="C14" t="n">
-        <v>0.806644806884698</v>
+        <v>0.821653548025072</v>
       </c>
       <c r="D14" t="n">
-        <v>-3.15151679670573</v>
+        <v>-3.19489973648341</v>
       </c>
       <c r="E14" t="n">
-        <v>1.51171548263862</v>
+        <v>1.5550984224163</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -1877,25 +1877,25 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>3.88050543051919</v>
+        <v>-2.28116311114461</v>
       </c>
       <c r="C4" t="n">
-        <v>0.76171110714712</v>
+        <v>0.351898043856357</v>
       </c>
       <c r="D4" t="n">
-        <v>1.66108773065704</v>
+        <v>-3.30649770289925</v>
       </c>
       <c r="E4" t="n">
-        <v>6.09992313038134</v>
+        <v>-1.25582851938997</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00000419687881524945</v>
+        <v>0.00000000108290656147483</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
@@ -1906,25 +1906,25 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-2.28116311114461</v>
+        <v>3.88050543051919</v>
       </c>
       <c r="C5" t="n">
-        <v>0.478519720602745</v>
+        <v>0.635089430400732</v>
       </c>
       <c r="D5" t="n">
-        <v>-3.67543861490682</v>
+        <v>2.03002864266461</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.886887607382393</v>
+        <v>5.73098221837376</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0000224248546027849</v>
+        <v>0.0000000119428849615354</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
@@ -1941,19 +1941,19 @@
         <v>-2.87261124480962</v>
       </c>
       <c r="C6" t="n">
-        <v>0.604863769991451</v>
+        <v>0.478242093245063</v>
       </c>
       <c r="D6" t="n">
-        <v>-4.63501873044063</v>
+        <v>-4.26607781843306</v>
       </c>
       <c r="E6" t="n">
-        <v>-1.1102037591786</v>
+        <v>-1.47914467118617</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0000245083049393418</v>
+        <v>0.0000000227338268801947</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
@@ -1970,19 +1970,19 @@
         <v>-4.27886174538928</v>
       </c>
       <c r="C7" t="n">
-        <v>0.901875304785586</v>
+        <v>0.775253628039198</v>
       </c>
       <c r="D7" t="n">
-        <v>-6.90667955679884</v>
+        <v>-6.53773864479127</v>
       </c>
       <c r="E7" t="n">
-        <v>-1.65104393397971</v>
+        <v>-2.01998484598729</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0000250944052996328</v>
+        <v>0.000000408410077974224</v>
       </c>
       <c r="H7" t="s">
         <v>26</v>
@@ -1999,112 +1999,112 @@
         <v>-2.02435170757185</v>
       </c>
       <c r="C8" t="n">
-        <v>0.518467313933071</v>
+        <v>0.391845637186683</v>
       </c>
       <c r="D8" t="n">
-        <v>-3.53502356537475</v>
+        <v>-3.16608265336718</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.513679849768952</v>
+        <v>-0.882620761776526</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.00113308012398904</v>
+        <v>0.00000286686174126159</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B9" t="n">
-        <v>2.68862406807983</v>
+        <v>-1.7448313110769</v>
       </c>
       <c r="C9" t="n">
-        <v>0.821113025597041</v>
+        <v>0.419913660508586</v>
       </c>
       <c r="D9" t="n">
-        <v>0.296125435070596</v>
+        <v>-2.96834479512888</v>
       </c>
       <c r="E9" t="n">
-        <v>5.08112270108906</v>
+        <v>-0.521317827024919</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0127079498546506</v>
+        <v>0.000389979098703508</v>
       </c>
       <c r="H9" t="s">
         <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.7448313110769</v>
+        <v>-2.10047574233186</v>
       </c>
       <c r="C10" t="n">
-        <v>0.546535337254974</v>
+        <v>0.534663915095059</v>
       </c>
       <c r="D10" t="n">
-        <v>-3.33728570713645</v>
+        <v>-3.65834006320801</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.152376915017345</v>
+        <v>-0.542611421455714</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0169237840330592</v>
+        <v>0.00102534103083569</v>
       </c>
       <c r="H10" t="s">
         <v>26</v>
       </c>
       <c r="I10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B11" t="n">
-        <v>-2.10047574233186</v>
+        <v>2.68862406807983</v>
       </c>
       <c r="C11" t="n">
-        <v>0.661285591841447</v>
+        <v>0.694491348850653</v>
       </c>
       <c r="D11" t="n">
-        <v>-4.02728097521559</v>
+        <v>0.66506634707817</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.173670509448141</v>
+        <v>4.71218178908149</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.017896790543035</v>
+        <v>0.00129877278194209</v>
       </c>
       <c r="H11" t="s">
         <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12">
@@ -2115,19 +2115,19 @@
         <v>-1.1043314014521</v>
       </c>
       <c r="C12" t="n">
-        <v>0.543197218499354</v>
+        <v>0.416575541752966</v>
       </c>
       <c r="D12" t="n">
-        <v>-2.68705943303967</v>
+        <v>-2.3181185210321</v>
       </c>
       <c r="E12" t="n">
-        <v>0.478396630135478</v>
+        <v>0.109455718127904</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.50460470737746</v>
+        <v>0.0963117009539047</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
@@ -2144,13 +2144,13 @@
         <v>0.737240752555557</v>
       </c>
       <c r="C13" t="n">
-        <v>0.912194718123191</v>
+        <v>0.785573041376803</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.92064500508556</v>
+        <v>-1.55170409307798</v>
       </c>
       <c r="E13" t="n">
-        <v>3.39512651019667</v>
+        <v>3.0261855981891</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -2173,13 +2173,13 @@
         <v>0.186861675188612</v>
       </c>
       <c r="C14" t="n">
-        <v>0.860007604761306</v>
+        <v>0.733385928014918</v>
       </c>
       <c r="D14" t="n">
-        <v>-2.31896511677208</v>
+        <v>-1.95002420476451</v>
       </c>
       <c r="E14" t="n">
-        <v>2.69268846714931</v>
+        <v>2.32374755514173</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -2202,13 +2202,13 @@
         <v>-0.337196087243825</v>
       </c>
       <c r="C15" t="n">
-        <v>0.646522053647952</v>
+        <v>0.519900376901564</v>
       </c>
       <c r="D15" t="n">
-        <v>-2.22098441034143</v>
+        <v>-1.85204349833385</v>
       </c>
       <c r="E15" t="n">
-        <v>1.54659223585378</v>
+        <v>1.1776513238462</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -2332,19 +2332,19 @@
         <v>-2.97705281260192</v>
       </c>
       <c r="C4" t="n">
-        <v>0.65887845702337</v>
+        <v>0.645069794567981</v>
       </c>
       <c r="D4" t="n">
-        <v>-4.91099250970462</v>
+        <v>-4.8704613309998</v>
       </c>
       <c r="E4" t="n">
-        <v>-1.04311311549921</v>
+        <v>-1.08364429420403</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.000081015001416609</v>
+        <v>0.000051081145091242</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
@@ -2361,19 +2361,19 @@
         <v>-2.36911056677888</v>
       </c>
       <c r="C5" t="n">
-        <v>0.553202369597206</v>
+        <v>0.539393707141817</v>
       </c>
       <c r="D5" t="n">
-        <v>-3.9928698681964</v>
+        <v>-3.95233868949158</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.745351265361361</v>
+        <v>-0.785882444066181</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.000240204857568503</v>
+        <v>0.00014589023435706</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -2390,19 +2390,19 @@
         <v>1.12619881795637</v>
       </c>
       <c r="C6" t="n">
-        <v>0.361311661051</v>
+        <v>0.34750299859561</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0656770223441343</v>
+        <v>0.106208201048954</v>
       </c>
       <c r="E6" t="n">
-        <v>2.18672061356861</v>
+        <v>2.14618943486379</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0237533516665213</v>
+        <v>0.0154935850975626</v>
       </c>
       <c r="H6" t="s">
         <v>10</v>
@@ -2419,19 +2419,19 @@
         <v>-1.34903800414999</v>
       </c>
       <c r="C7" t="n">
-        <v>0.514517520050126</v>
+        <v>0.500708857594736</v>
       </c>
       <c r="D7" t="n">
-        <v>-2.85924955572374</v>
+        <v>-2.81871837701892</v>
       </c>
       <c r="E7" t="n">
-        <v>0.161173547423747</v>
+        <v>0.120642368718928</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.113657516207731</v>
+        <v>0.0917096570364839</v>
       </c>
       <c r="H7" t="s">
         <v>10</v>
@@ -2448,19 +2448,19 @@
         <v>-1.31254760567531</v>
       </c>
       <c r="C8" t="n">
-        <v>0.548323545881458</v>
+        <v>0.534514883426069</v>
       </c>
       <c r="D8" t="n">
-        <v>-2.92198658631367</v>
+        <v>-2.88145540760885</v>
       </c>
       <c r="E8" t="n">
-        <v>0.296891374963048</v>
+        <v>0.256360196258229</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.216804480509727</v>
+        <v>0.182851296535574</v>
       </c>
       <c r="H8" t="s">
         <v>10</v>
@@ -2477,19 +2477,19 @@
         <v>1.34611942528998</v>
       </c>
       <c r="C9" t="n">
-        <v>0.609443961831876</v>
+        <v>0.595635299376487</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.442720167782961</v>
+        <v>-0.402188989078142</v>
       </c>
       <c r="E9" t="n">
-        <v>3.13495901836292</v>
+        <v>3.0944278396581</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.35348149374962</v>
+        <v>0.309698410565498</v>
       </c>
       <c r="H9" t="s">
         <v>10</v>
@@ -2506,19 +2506,19 @@
         <v>1.12563245824976</v>
       </c>
       <c r="C10" t="n">
-        <v>0.616479004893028</v>
+        <v>0.602670342437638</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.683856389479728</v>
+        <v>-0.643325210774909</v>
       </c>
       <c r="E10" t="n">
-        <v>2.93512130597924</v>
+        <v>2.89459012727442</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.882238301715663</v>
+        <v>0.803375297133251</v>
       </c>
       <c r="H10" t="s">
         <v>10</v>
@@ -2535,13 +2535,13 @@
         <v>-0.409649207409245</v>
       </c>
       <c r="C11" t="n">
-        <v>0.56479190232788</v>
+        <v>0.550983239872491</v>
       </c>
       <c r="D11" t="n">
-        <v>-2.06742609914225</v>
+        <v>-2.02689492043743</v>
       </c>
       <c r="E11" t="n">
-        <v>1.24812768432376</v>
+        <v>1.20759650561894</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -2564,13 +2564,13 @@
         <v>0.0907686684785104</v>
       </c>
       <c r="C12" t="n">
-        <v>0.347391128276737</v>
+        <v>0.333582465821347</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.928893586728371</v>
+        <v>-0.888362408023552</v>
       </c>
       <c r="E12" t="n">
-        <v>1.11043092368539</v>
+        <v>1.06989974498057</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -2593,13 +2593,13 @@
         <v>-0.274703212183046</v>
       </c>
       <c r="C13" t="n">
-        <v>0.344330181578696</v>
+        <v>0.330521519123307</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.28538097826761</v>
+        <v>-1.24484979956279</v>
       </c>
       <c r="E13" t="n">
-        <v>0.735974553901517</v>
+        <v>0.695443375196698</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -2622,13 +2622,13 @@
         <v>0.00526298379007351</v>
       </c>
       <c r="C14" t="n">
-        <v>0.235744963373115</v>
+        <v>0.221936300917725</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.686695507490692</v>
+        <v>-0.646164328785873</v>
       </c>
       <c r="E14" t="n">
-        <v>0.697221475070839</v>
+        <v>0.65669029636602</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -2651,13 +2651,13 @@
         <v>-0.108883874006839</v>
       </c>
       <c r="C15" t="n">
-        <v>0.40426316911106</v>
+        <v>0.39045450665567</v>
       </c>
       <c r="D15" t="n">
-        <v>-1.29547691326399</v>
+        <v>-1.25494573455917</v>
       </c>
       <c r="E15" t="n">
-        <v>1.07770916525031</v>
+        <v>1.03717798654549</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -2680,13 +2680,13 @@
         <v>0.219364407734019</v>
       </c>
       <c r="C16" t="n">
-        <v>0.306334400333686</v>
+        <v>0.292525737878296</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.679788161421014</v>
+        <v>-0.639256982716194</v>
       </c>
       <c r="E16" t="n">
-        <v>1.11851697688905</v>
+        <v>1.07798579818423</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -2810,19 +2810,19 @@
         <v>-1.65084418948903</v>
       </c>
       <c r="C3" t="n">
-        <v>0.814155925898332</v>
+        <v>0.759335571046395</v>
       </c>
       <c r="D3" t="n">
-        <v>-4.02307173800686</v>
+        <v>-3.86334022729435</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7213833590288</v>
+        <v>0.561651848316287</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5537136409522</v>
+        <v>0.386104200571638</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
@@ -2839,19 +2839,19 @@
         <v>1.66884383726834</v>
       </c>
       <c r="C4" t="n">
-        <v>0.888160866343194</v>
+        <v>0.833340511491258</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.919013853910447</v>
+        <v>-0.759282343197933</v>
       </c>
       <c r="E4" t="n">
-        <v>4.25670152844713</v>
+        <v>4.09697001773462</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.783199258548616</v>
+        <v>0.587869605413677</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
@@ -2868,13 +2868,13 @@
         <v>-0.673126139068271</v>
       </c>
       <c r="C5" t="n">
-        <v>0.579285769126771</v>
+        <v>0.524465414274835</v>
       </c>
       <c r="D5" t="n">
-        <v>-2.36100633040949</v>
+        <v>-2.20127481969698</v>
       </c>
       <c r="E5" t="n">
-        <v>1.01475405227295</v>
+        <v>0.855022541560436</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -2897,13 +2897,13 @@
         <v>0.204938049276485</v>
       </c>
       <c r="C6" t="n">
-        <v>0.512065472444708</v>
+        <v>0.457245117592772</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.28708059449597</v>
+        <v>-1.12734908378345</v>
       </c>
       <c r="E6" t="n">
-        <v>1.69695669304894</v>
+        <v>1.53722518233642</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -2926,13 +2926,13 @@
         <v>0.699231034828448</v>
       </c>
       <c r="C7" t="n">
-        <v>0.730955744869076</v>
+        <v>0.676135390017139</v>
       </c>
       <c r="D7" t="n">
-        <v>-1.43057395653426</v>
+        <v>-1.27084244582174</v>
       </c>
       <c r="E7" t="n">
-        <v>2.82903602619115</v>
+        <v>2.66930451547864</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -2955,13 +2955,13 @@
         <v>0.656919424047354</v>
       </c>
       <c r="C8" t="n">
-        <v>0.747958874038453</v>
+        <v>0.693138519186517</v>
       </c>
       <c r="D8" t="n">
-        <v>-1.5224280322702</v>
+        <v>-1.36269652155769</v>
       </c>
       <c r="E8" t="n">
-        <v>2.83626688036491</v>
+        <v>2.6765353696524</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -2984,13 +2984,13 @@
         <v>0.00541284716531187</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4662472790578</v>
+        <v>0.411426924205864</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.35310412067718</v>
+        <v>-1.19337260996466</v>
       </c>
       <c r="E9" t="n">
-        <v>1.3639298150078</v>
+        <v>1.20419830429529</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -3013,13 +3013,13 @@
         <v>-0.978614048590889</v>
       </c>
       <c r="C10" t="n">
-        <v>0.765019707036194</v>
+        <v>0.710199352184258</v>
       </c>
       <c r="D10" t="n">
-        <v>-3.20767210302667</v>
+        <v>-3.04794059231416</v>
       </c>
       <c r="E10" t="n">
-        <v>1.2504440058449</v>
+        <v>1.09071249513238</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -3042,13 +3042,13 @@
         <v>-0.781037226566709</v>
       </c>
       <c r="C11" t="n">
-        <v>0.820655826372363</v>
+        <v>0.765835471520427</v>
       </c>
       <c r="D11" t="n">
-        <v>-3.17220370616228</v>
+        <v>-3.01247219544977</v>
       </c>
       <c r="E11" t="n">
-        <v>1.61012925302886</v>
+        <v>1.45039774231635</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -3071,13 +3071,13 @@
         <v>-0.142316177794834</v>
       </c>
       <c r="C12" t="n">
-        <v>0.511261337827635</v>
+        <v>0.456440982975699</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.63199179337004</v>
+        <v>-1.47226028265752</v>
       </c>
       <c r="E12" t="n">
-        <v>1.34735943778037</v>
+        <v>1.18762792706785</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -3100,13 +3100,13 @@
         <v>1.65250752118857</v>
       </c>
       <c r="C13" t="n">
-        <v>1.08243045383996</v>
+        <v>1.02761009898802</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.5013985799315</v>
+        <v>-1.34166706921899</v>
       </c>
       <c r="E13" t="n">
-        <v>4.80641362230864</v>
+        <v>4.64668211159613</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -3129,13 +3129,13 @@
         <v>-0.634087549662734</v>
       </c>
       <c r="C14" t="n">
-        <v>0.453220833622229</v>
+        <v>0.398400478770293</v>
       </c>
       <c r="D14" t="n">
-        <v>-1.95464902060525</v>
+        <v>-1.79491750989274</v>
       </c>
       <c r="E14" t="n">
-        <v>0.686473921279782</v>
+        <v>0.526742410567268</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -3158,13 +3158,13 @@
         <v>-0.399979368736203</v>
       </c>
       <c r="C15" t="n">
-        <v>0.461856487466222</v>
+        <v>0.407036132614286</v>
       </c>
       <c r="D15" t="n">
-        <v>-1.74570277155999</v>
+        <v>-1.58597126084747</v>
       </c>
       <c r="E15" t="n">
-        <v>0.945744034087581</v>
+        <v>0.786012523375067</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>

</xml_diff>